<commit_message>
Added cancelamentos and statusTime
</commit_message>
<xml_diff>
--- a/files/MarineTraffic_ExpectedArrivalExport_2022-07-31.xlsx
+++ b/files/MarineTraffic_ExpectedArrivalExport_2022-07-31.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.catossi\source\repos\zwt-api\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E417E37F-1AE2-4F57-8936-382D6D459290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3696567C-70B1-4C42-84F7-95716C15A1B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="250">
   <si>
     <t>Reported Eta</t>
   </si>
@@ -94,9 +94,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>ASL URANUS</t>
-  </si>
-  <si>
     <t>SANTOS</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>5LAC6</t>
   </si>
   <si>
-    <t>YARA</t>
-  </si>
-  <si>
     <t>Tanker</t>
   </si>
   <si>
@@ -337,9 +331,6 @@
     <t>V7NW9</t>
   </si>
   <si>
-    <t>THE STRONG</t>
-  </si>
-  <si>
     <t>Arabian Gulf</t>
   </si>
   <si>
@@ -385,9 +376,6 @@
     <t>V7A2409</t>
   </si>
   <si>
-    <t>TINOS</t>
-  </si>
-  <si>
     <t>D5IV6</t>
   </si>
   <si>
@@ -400,9 +388,6 @@
     <t>D5RN5</t>
   </si>
   <si>
-    <t>FORTUNE SUN</t>
-  </si>
-  <si>
     <t>SANTOS,BRAZIL</t>
   </si>
   <si>
@@ -436,9 +421,6 @@
     <t>V7A2444</t>
   </si>
   <si>
-    <t>LEGIO X EQUESTRIS</t>
-  </si>
-  <si>
     <t>SGSIN &gt; FOR ORDERS</t>
   </si>
   <si>
@@ -466,9 +448,6 @@
     <t>5BPP3</t>
   </si>
   <si>
-    <t>ADVANCE</t>
-  </si>
-  <si>
     <t>10.7</t>
   </si>
   <si>
@@ -481,9 +460,6 @@
     <t>3FTS7</t>
   </si>
   <si>
-    <t>MOTTLER</t>
-  </si>
-  <si>
     <t>MONTREAL</t>
   </si>
   <si>
@@ -625,9 +601,6 @@
     <t>3FYV3</t>
   </si>
   <si>
-    <t>MARITIME JINGAN</t>
-  </si>
-  <si>
     <t>180.0</t>
   </si>
   <si>
@@ -773,6 +746,30 @@
   </si>
   <si>
     <t>2022-07-31 12:00:00.007</t>
+  </si>
+  <si>
+    <t>MAERSK VENTURE</t>
+  </si>
+  <si>
+    <t>MSC ALICANTE</t>
+  </si>
+  <si>
+    <t>NORMAND MARINER</t>
+  </si>
+  <si>
+    <t>SANTA VICTORIA</t>
+  </si>
+  <si>
+    <t>MAERSK LIMA</t>
+  </si>
+  <si>
+    <t>BOW OCEANIC</t>
+  </si>
+  <si>
+    <t>OVERSEAS MILOS</t>
+  </si>
+  <si>
+    <t>NEDLLOYD HONSHU</t>
   </si>
 </sst>
 </file>
@@ -1625,8 +1622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,22 +1728,22 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>249</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="F2">
         <v>82372</v>
       </c>
       <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
         <v>26</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
       </c>
       <c r="I2">
         <v>9317511</v>
@@ -1755,31 +1752,31 @@
         <v>636020665</v>
       </c>
       <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
         <v>28</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>29</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>30</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>31</v>
-      </c>
-      <c r="R2" t="s">
-        <v>32</v>
       </c>
       <c r="S2">
         <v>2008</v>
       </c>
       <c r="T2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U2" t="s">
         <v>33</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>34</v>
-      </c>
-      <c r="V2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -1787,22 +1784,22 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>246</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="F3">
         <v>21181</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I3">
         <v>9276248</v>
@@ -1811,31 +1808,31 @@
         <v>574005110</v>
       </c>
       <c r="M3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" t="s">
         <v>28</v>
       </c>
-      <c r="N3" t="s">
-        <v>29</v>
-      </c>
       <c r="O3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="S3">
         <v>2003</v>
       </c>
       <c r="T3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V3" t="s">
         <v>41</v>
-      </c>
-      <c r="U3" t="s">
-        <v>42</v>
-      </c>
-      <c r="V3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -1843,22 +1840,22 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="F4">
         <v>81984</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I4">
         <v>9864083</v>
@@ -1870,31 +1867,31 @@
         <v>357762000</v>
       </c>
       <c r="M4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" t="s">
         <v>46</v>
       </c>
-      <c r="N4" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" t="s">
-        <v>48</v>
-      </c>
       <c r="R4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S4">
         <v>2020</v>
       </c>
       <c r="T4" t="s">
+        <v>47</v>
+      </c>
+      <c r="U4" t="s">
+        <v>48</v>
+      </c>
+      <c r="V4" t="s">
         <v>49</v>
-      </c>
-      <c r="U4" t="s">
-        <v>50</v>
-      </c>
-      <c r="V4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -1902,22 +1899,22 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="F5">
         <v>81068</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I5">
         <v>9611553</v>
@@ -1926,31 +1923,31 @@
         <v>566832000</v>
       </c>
       <c r="M5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N5" t="s">
+        <v>52</v>
+      </c>
+      <c r="O5" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" t="s">
         <v>54</v>
       </c>
-      <c r="O5" t="s">
-        <v>55</v>
-      </c>
-      <c r="P5" t="s">
-        <v>56</v>
-      </c>
       <c r="R5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S5">
         <v>2013</v>
       </c>
       <c r="T5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -1958,22 +1955,22 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="F6">
         <v>81964</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I6">
         <v>9628934</v>
@@ -1985,31 +1982,31 @@
         <v>241222000</v>
       </c>
       <c r="M6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" t="s">
         <v>28</v>
       </c>
-      <c r="N6" t="s">
-        <v>29</v>
-      </c>
       <c r="O6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S6">
         <v>2013</v>
       </c>
       <c r="T6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -2017,22 +2014,22 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="F7">
         <v>79791</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I7">
         <v>9469510</v>
@@ -2041,31 +2038,31 @@
         <v>256786000</v>
       </c>
       <c r="M7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S7">
         <v>2011</v>
       </c>
       <c r="T7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -2073,22 +2070,22 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="F8">
         <v>63993</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I8">
         <v>9802229</v>
@@ -2100,31 +2097,31 @@
         <v>538008776</v>
       </c>
       <c r="M8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" t="s">
         <v>28</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>29</v>
       </c>
-      <c r="O8" t="s">
-        <v>30</v>
-      </c>
       <c r="P8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="R8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S8">
         <v>2020</v>
       </c>
       <c r="T8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="U8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -2132,22 +2129,22 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="F9">
         <v>82384</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I9">
         <v>9934943</v>
@@ -2159,31 +2156,31 @@
         <v>352001206</v>
       </c>
       <c r="M9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="R9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S9">
         <v>2022</v>
       </c>
       <c r="T9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -2191,22 +2188,22 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="F10">
         <v>85015</v>
       </c>
       <c r="G10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I10">
         <v>9738222</v>
@@ -2218,31 +2215,31 @@
         <v>538007177</v>
       </c>
       <c r="M10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" t="s">
         <v>28</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>29</v>
       </c>
-      <c r="O10" t="s">
-        <v>30</v>
-      </c>
       <c r="P10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S10">
         <v>2017</v>
       </c>
       <c r="T10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="V10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -2250,22 +2247,22 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F11">
         <v>70663</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I11">
         <v>9609469</v>
@@ -2274,31 +2271,31 @@
         <v>229308000</v>
       </c>
       <c r="M11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N11" t="s">
         <v>28</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>29</v>
       </c>
-      <c r="O11" t="s">
-        <v>30</v>
-      </c>
       <c r="P11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S11">
         <v>2013</v>
       </c>
       <c r="T11" t="s">
+        <v>78</v>
+      </c>
+      <c r="U11" t="s">
+        <v>79</v>
+      </c>
+      <c r="V11" t="s">
         <v>80</v>
-      </c>
-      <c r="U11" t="s">
-        <v>81</v>
-      </c>
-      <c r="V11" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -2306,22 +2303,22 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F12">
         <v>74500</v>
       </c>
       <c r="G12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" t="s">
         <v>26</v>
-      </c>
-      <c r="H12" t="s">
-        <v>27</v>
       </c>
       <c r="I12">
         <v>9357755</v>
@@ -2330,31 +2327,31 @@
         <v>636020274</v>
       </c>
       <c r="M12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N12" t="s">
         <v>28</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>29</v>
       </c>
-      <c r="O12" t="s">
-        <v>30</v>
-      </c>
       <c r="P12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="R12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S12">
         <v>2008</v>
       </c>
       <c r="T12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="U12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -2362,22 +2359,22 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="F13">
         <v>64000</v>
       </c>
       <c r="G13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I13">
         <v>9766932</v>
@@ -2389,31 +2386,31 @@
         <v>352001327</v>
       </c>
       <c r="M13" t="s">
+        <v>86</v>
+      </c>
+      <c r="N13" t="s">
+        <v>86</v>
+      </c>
+      <c r="O13" t="s">
+        <v>87</v>
+      </c>
+      <c r="P13" t="s">
         <v>88</v>
       </c>
-      <c r="N13" t="s">
-        <v>88</v>
-      </c>
-      <c r="O13" t="s">
-        <v>89</v>
-      </c>
-      <c r="P13" t="s">
-        <v>90</v>
-      </c>
       <c r="R13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S13">
         <v>2017</v>
       </c>
       <c r="T13" t="s">
+        <v>89</v>
+      </c>
+      <c r="U13" t="s">
+        <v>90</v>
+      </c>
+      <c r="V13" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="U13" t="s">
-        <v>92</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -2421,22 +2418,22 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="F14">
         <v>78208</v>
       </c>
       <c r="G14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I14">
         <v>9840673</v>
@@ -2448,31 +2445,31 @@
         <v>477468900</v>
       </c>
       <c r="M14" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" t="s">
         <v>28</v>
       </c>
-      <c r="N14" t="s">
-        <v>29</v>
-      </c>
       <c r="O14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S14">
         <v>2020</v>
       </c>
       <c r="T14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="U14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -2480,22 +2477,22 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="F15">
         <v>82010</v>
       </c>
       <c r="G15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I15">
         <v>9827401</v>
@@ -2507,31 +2504,31 @@
         <v>311000759</v>
       </c>
       <c r="M15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S15">
         <v>2019</v>
       </c>
       <c r="T15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
@@ -2539,22 +2536,22 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="F16">
         <v>81502</v>
       </c>
       <c r="G16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I16">
         <v>9597757</v>
@@ -2563,31 +2560,31 @@
         <v>538007443</v>
       </c>
       <c r="M16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="R16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S16">
         <v>2011</v>
       </c>
       <c r="T16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
@@ -2595,22 +2592,22 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>105</v>
+        <v>247</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F17">
         <v>74823</v>
       </c>
       <c r="G17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I17">
         <v>9287455</v>
@@ -2619,31 +2616,31 @@
         <v>356499000</v>
       </c>
       <c r="M17" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="O17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S17">
         <v>2004</v>
       </c>
       <c r="T17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="U17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
@@ -2651,22 +2648,22 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="F18">
         <v>79528</v>
       </c>
       <c r="G18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I18">
         <v>9474694</v>
@@ -2675,31 +2672,31 @@
         <v>538005619</v>
       </c>
       <c r="M18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P18" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S18">
         <v>2014</v>
       </c>
       <c r="T18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
@@ -2707,22 +2704,22 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="F19">
         <v>106043</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I19">
         <v>9526904</v>
@@ -2731,31 +2728,31 @@
         <v>477764700</v>
       </c>
       <c r="M19" t="s">
+        <v>27</v>
+      </c>
+      <c r="N19" t="s">
         <v>28</v>
       </c>
-      <c r="N19" t="s">
-        <v>29</v>
-      </c>
       <c r="O19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="P19" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="R19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S19">
         <v>2011</v>
       </c>
       <c r="T19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="U19" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="V19" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
@@ -2763,22 +2760,22 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="F20">
         <v>81834</v>
       </c>
       <c r="G20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I20">
         <v>9837016</v>
@@ -2790,31 +2787,31 @@
         <v>538008482</v>
       </c>
       <c r="M20" t="s">
+        <v>27</v>
+      </c>
+      <c r="N20" t="s">
         <v>28</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>29</v>
       </c>
-      <c r="O20" t="s">
-        <v>30</v>
-      </c>
       <c r="P20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="R20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S20">
         <v>2019</v>
       </c>
       <c r="T20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V20" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
@@ -2822,22 +2819,22 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>121</v>
+        <v>245</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="F21">
         <v>81391</v>
       </c>
       <c r="G21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" t="s">
         <v>26</v>
-      </c>
-      <c r="H21" t="s">
-        <v>27</v>
       </c>
       <c r="I21">
         <v>9597795</v>
@@ -2846,31 +2843,31 @@
         <v>636017003</v>
       </c>
       <c r="M21" t="s">
+        <v>27</v>
+      </c>
+      <c r="N21" t="s">
         <v>28</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>29</v>
       </c>
-      <c r="O21" t="s">
-        <v>30</v>
-      </c>
       <c r="P21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="R21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S21">
         <v>2011</v>
       </c>
       <c r="T21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V21" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
@@ -2878,22 +2875,22 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="F22">
         <v>75118</v>
       </c>
       <c r="G22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" t="s">
         <v>26</v>
-      </c>
-      <c r="H22" t="s">
-        <v>27</v>
       </c>
       <c r="I22">
         <v>9422328</v>
@@ -2902,31 +2899,31 @@
         <v>636018819</v>
       </c>
       <c r="M22" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N22" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="O22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="R22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S22">
         <v>2008</v>
       </c>
       <c r="T22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="U22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V22" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
@@ -2934,22 +2931,22 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>126</v>
+        <v>242</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="F23">
         <v>74193</v>
       </c>
       <c r="G23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I23">
         <v>9267211</v>
@@ -2958,31 +2955,31 @@
         <v>538004103</v>
       </c>
       <c r="M23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O23" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="P23" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="R23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S23">
         <v>2002</v>
       </c>
       <c r="T23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U23" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="V23" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
@@ -2990,22 +2987,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="F24">
         <v>81804</v>
       </c>
       <c r="G24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I24">
         <v>9596090</v>
@@ -3017,31 +3014,31 @@
         <v>371089000</v>
       </c>
       <c r="M24" t="s">
+        <v>27</v>
+      </c>
+      <c r="N24" t="s">
         <v>28</v>
       </c>
-      <c r="N24" t="s">
-        <v>29</v>
-      </c>
       <c r="O24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="R24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S24">
         <v>2013</v>
       </c>
       <c r="T24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U24" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="V24" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
@@ -3049,22 +3046,22 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="F25">
         <v>80000</v>
       </c>
       <c r="G25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I25">
         <v>9867140</v>
@@ -3076,28 +3073,28 @@
         <v>538008507</v>
       </c>
       <c r="M25" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="N25" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="O25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P25" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="R25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V25" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
@@ -3105,22 +3102,22 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="F26">
         <v>299937</v>
       </c>
       <c r="G26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I26">
         <v>9912256</v>
@@ -3132,31 +3129,31 @@
         <v>538009642</v>
       </c>
       <c r="M26" t="s">
+        <v>27</v>
+      </c>
+      <c r="N26" t="s">
         <v>28</v>
       </c>
-      <c r="N26" t="s">
-        <v>29</v>
-      </c>
       <c r="O26" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="P26" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="R26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S26">
         <v>2022</v>
       </c>
       <c r="T26" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="U26" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="V26" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
@@ -3164,22 +3161,22 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F27">
         <v>81391</v>
       </c>
       <c r="G27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H27" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I27">
         <v>9627057</v>
@@ -3188,31 +3185,31 @@
         <v>212384000</v>
       </c>
       <c r="M27" t="s">
+        <v>27</v>
+      </c>
+      <c r="N27" t="s">
         <v>28</v>
       </c>
-      <c r="N27" t="s">
-        <v>29</v>
-      </c>
       <c r="O27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="P27" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="R27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S27">
         <v>2012</v>
       </c>
       <c r="T27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V27" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
@@ -3220,22 +3217,22 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>148</v>
+        <v>244</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="F28">
         <v>25925</v>
       </c>
       <c r="G28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I28">
         <v>9149859</v>
@@ -3244,31 +3241,31 @@
         <v>351645000</v>
       </c>
       <c r="M28" t="s">
+        <v>27</v>
+      </c>
+      <c r="N28" t="s">
         <v>28</v>
       </c>
-      <c r="N28" t="s">
-        <v>29</v>
-      </c>
       <c r="O28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="P28" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="R28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S28">
         <v>1997</v>
       </c>
       <c r="T28" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="U28" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="V28" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
@@ -3276,22 +3273,22 @@
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>153</v>
+        <v>248</v>
       </c>
       <c r="C29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="F29">
         <v>30806</v>
       </c>
       <c r="G29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I29">
         <v>9477828</v>
@@ -3300,40 +3297,40 @@
         <v>212735000</v>
       </c>
       <c r="L29" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="M29" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="N29" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="O29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P29" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="Q29" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="R29" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="S29">
         <v>2009</v>
       </c>
       <c r="T29" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="U29" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="V29" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="W29" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
@@ -3341,22 +3338,22 @@
         <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="F30">
         <v>81434</v>
       </c>
       <c r="G30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I30">
         <v>9628087</v>
@@ -3365,31 +3362,31 @@
         <v>229026000</v>
       </c>
       <c r="M30" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="N30" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="O30" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="P30" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="R30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S30">
         <v>2013</v>
       </c>
       <c r="T30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V30" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
@@ -3397,22 +3394,22 @@
         <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="F31">
         <v>50779</v>
       </c>
       <c r="G31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I31">
         <v>9401934</v>
@@ -3421,31 +3418,31 @@
         <v>229725000</v>
       </c>
       <c r="M31" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="N31" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="O31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="R31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S31">
         <v>2010</v>
       </c>
       <c r="T31" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="U31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V31" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
@@ -3453,22 +3450,22 @@
         <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="F32">
         <v>57266</v>
       </c>
       <c r="G32" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" t="s">
         <v>26</v>
-      </c>
-      <c r="H32" t="s">
-        <v>27</v>
       </c>
       <c r="I32">
         <v>9451173</v>
@@ -3477,31 +3474,31 @@
         <v>636021074</v>
       </c>
       <c r="M32" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="N32" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="O32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S32">
         <v>2010</v>
       </c>
       <c r="T32" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="U32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V32" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
@@ -3509,22 +3506,22 @@
         <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="F33">
         <v>49746</v>
       </c>
       <c r="G33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I33">
         <v>9692301</v>
@@ -3533,31 +3530,31 @@
         <v>538006226</v>
       </c>
       <c r="M33" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="N33" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="O33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P33" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="R33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S33">
         <v>2015</v>
       </c>
       <c r="T33" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="U33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V33" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
@@ -3565,22 +3562,22 @@
         <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="F34">
         <v>38134</v>
       </c>
       <c r="G34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I34">
         <v>9704752</v>
@@ -3589,31 +3586,31 @@
         <v>477915600</v>
       </c>
       <c r="M34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P34" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="R34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S34">
         <v>2016</v>
       </c>
       <c r="T34" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="U34" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="V34" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
@@ -3621,22 +3618,22 @@
         <v>23</v>
       </c>
       <c r="B35" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="F35">
         <v>128653</v>
       </c>
       <c r="G35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H35" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="I35">
         <v>9622239</v>
@@ -3645,40 +3642,40 @@
         <v>219100000</v>
       </c>
       <c r="L35" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="M35" t="s">
+        <v>160</v>
+      </c>
+      <c r="N35" t="s">
+        <v>177</v>
+      </c>
+      <c r="O35" t="s">
+        <v>178</v>
+      </c>
+      <c r="P35" t="s">
         <v>168</v>
       </c>
-      <c r="N35" t="s">
-        <v>185</v>
-      </c>
-      <c r="O35" t="s">
-        <v>186</v>
-      </c>
-      <c r="P35" t="s">
-        <v>176</v>
-      </c>
       <c r="Q35" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="R35" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="S35">
         <v>2013</v>
       </c>
       <c r="T35" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="U35" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="V35" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="W35" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
@@ -3686,22 +3683,22 @@
         <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="F36">
         <v>81117</v>
       </c>
       <c r="G36" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36" t="s">
         <v>26</v>
-      </c>
-      <c r="H36" t="s">
-        <v>27</v>
       </c>
       <c r="I36">
         <v>9841160</v>
@@ -3713,31 +3710,31 @@
         <v>636019940</v>
       </c>
       <c r="M36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N36" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S36">
         <v>2018</v>
       </c>
       <c r="T36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V36" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
@@ -3745,22 +3742,22 @@
         <v>23</v>
       </c>
       <c r="B37" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="F37">
         <v>39763</v>
       </c>
       <c r="G37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I37">
         <v>9307425</v>
@@ -3769,31 +3766,31 @@
         <v>563152400</v>
       </c>
       <c r="M37" t="s">
+        <v>27</v>
+      </c>
+      <c r="N37" t="s">
         <v>28</v>
       </c>
-      <c r="N37" t="s">
-        <v>29</v>
-      </c>
       <c r="O37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="P37" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="R37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S37">
         <v>2006</v>
       </c>
       <c r="T37" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="U37" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="V37" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
@@ -3801,22 +3798,22 @@
         <v>23</v>
       </c>
       <c r="B38" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="F38">
         <v>82000</v>
       </c>
       <c r="G38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H38" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I38">
         <v>9611565</v>
@@ -3825,31 +3822,31 @@
         <v>352614000</v>
       </c>
       <c r="M38" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="N38" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="O38" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="P38" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="R38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S38">
         <v>2013</v>
       </c>
       <c r="T38" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V38" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
@@ -3857,22 +3854,22 @@
         <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>201</v>
+        <v>243</v>
       </c>
       <c r="C39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="F39">
         <v>44411</v>
       </c>
       <c r="G39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H39" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I39">
         <v>9251523</v>
@@ -3881,31 +3878,31 @@
         <v>477277000</v>
       </c>
       <c r="M39" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="N39" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="O39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P39" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="R39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S39">
         <v>2003</v>
       </c>
       <c r="T39" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="U39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V39" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
@@ -3913,22 +3910,22 @@
         <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="F40">
         <v>74823</v>
       </c>
       <c r="G40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H40" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I40">
         <v>9280770</v>
@@ -3937,31 +3934,31 @@
         <v>538002838</v>
       </c>
       <c r="M40" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N40" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="O40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P40" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="R40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S40">
         <v>2004</v>
       </c>
       <c r="T40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="U40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V40" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
@@ -3969,22 +3966,22 @@
         <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="F41">
         <v>57440</v>
       </c>
       <c r="G41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I41">
         <v>9613329</v>
@@ -3993,31 +3990,31 @@
         <v>538005205</v>
       </c>
       <c r="M41" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="N41" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="O41" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="P41" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="R41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S41">
         <v>2013</v>
       </c>
       <c r="T41" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="U41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V41" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>